<commit_message>
Creation de toutes les tables fini, il ne reste plus que l'insertion des données
</commit_message>
<xml_diff>
--- a/MLD & cartes/Splendor_Cartes - sans requetes.xlsx
+++ b/MLD & cartes/Splendor_Cartes - sans requetes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Cours\2018-2019\MA-24\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Ma24\Splendor\MLD &amp; cartes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Niveau (1 à 3, 4==noble)</t>
   </si>
@@ -33,21 +33,6 @@
   </si>
   <si>
     <t>Points prestige</t>
-  </si>
-  <si>
-    <t>Coût Rubis (1)</t>
-  </si>
-  <si>
-    <t>Coût Emeraude (2)</t>
-  </si>
-  <si>
-    <t>Coût Onyx (3)</t>
-  </si>
-  <si>
-    <t>Coût Saphir (4)</t>
-  </si>
-  <si>
-    <t>Coût Diamant (5)</t>
   </si>
 </sst>
 </file>
@@ -381,32 +366,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="62.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875"/>
-    <col min="13" max="13" width="29.44140625" customWidth="1"/>
-    <col min="14" max="1025" width="11.5546875"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="90.28515625" customWidth="1"/>
+    <col min="10" max="10" width="86.7109375" customWidth="1"/>
+    <col min="11" max="11" width="81.5703125" customWidth="1"/>
+    <col min="12" max="12" width="75.140625" customWidth="1"/>
+    <col min="13" max="13" width="81.42578125" customWidth="1"/>
+    <col min="14" max="14" width="71.28515625" customWidth="1"/>
+    <col min="15" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,23 +402,23 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4</v>
       </c>
@@ -446,11 +432,31 @@
         <v>4</v>
       </c>
       <c r="I2" t="str">
-        <f>"insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", 0,"&amp;A2&amp;","&amp;C2&amp;")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (2, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <f>"DoSqlRequest(""insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", "&amp;B2&amp;","&amp;A2&amp;","&amp;C2&amp;")"");"</f>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (2, ,4,3)");</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(ISBLANK(D2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D2),0,D2)&amp;")"")")</f>
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:N2" si="0">IF(ISBLANK(E2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E2),0,E2)&amp;")"")")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(2, 2, 4)")</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(2, 4, 4)")</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -464,11 +470,31 @@
         <v>4</v>
       </c>
       <c r="I3" t="str">
-        <f>"insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", 0,"&amp;A3&amp;","&amp;C3&amp;")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (3, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I66" si="1">"DoSqlRequest(""insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", "&amp;B3&amp;","&amp;A3&amp;","&amp;C3&amp;")"");"</f>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (3, ,4,3)");</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="2">IF(ISBLANK(D3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D3),0,D3)&amp;")"")")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(3, 1, 4)")</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="3">IF(ISBLANK(E3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E3),0,E3)&amp;")"")")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(3, 2, 4)")</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L66" si="4">IF(ISBLANK(F3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F3),0,F3)&amp;")"")")</f>
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M66" si="5">IF(ISBLANK(G3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G3),0,G3)&amp;")"")")</f>
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N66" si="6">IF(ISBLANK(H3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H3),0,H3)&amp;")"")")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -485,11 +511,31 @@
         <v>3</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I11" si="0">"insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", 0,"&amp;A4&amp;","&amp;C4&amp;")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (4, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (4, ,4,3)");</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 3, 3)")</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 4, 3)")</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -503,11 +549,31 @@
         <v>4</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (5, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (5, ,4,3)");</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(5, 3, 4)")</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(5, 5, 4)")</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -521,11 +587,31 @@
         <v>4</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (6, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (6, ,4,3)");</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(6, 1, 4)")</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(6, 3, 4)")</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -542,11 +628,31 @@
         <v>3</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (7, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (7, ,4,3)");</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 1, 3)")</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 3, 3)")</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -563,11 +669,31 @@
         <v>3</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (8, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (8, ,4,3)");</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 2, 3)")</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 4, 3)")</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -584,11 +710,31 @@
         <v>3</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (9, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (9, ,4,3)");</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 1, 3)")</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 2, 3)")</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 4, 3)")</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -602,11 +748,31 @@
         <v>4</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (10, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (10, ,4,3)");</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(10, 4, 4)")</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(10, 5, 4)")</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -623,11 +789,31 @@
         <v>3</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (11, 0,4,3)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (11, ,4,3)");</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 1, 3)")</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 2, 3)")</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 3, 3)")</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -644,11 +830,31 @@
         <v>7</v>
       </c>
       <c r="I12" t="str">
-        <f>"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B12 &amp; "," &amp; A12 &amp; "," &amp; C12 &amp; ")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (12,4,3,5)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (12, 4,3,5)");</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(12, 4, 3)")</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(12, 5, 7)")</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -665,11 +871,31 @@
         <v>3</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I76" si="1">"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B13 &amp; "," &amp; A13 &amp; "," &amp; C13 &amp; ")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (13,3,3,5)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (13, 3,3,5)");</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(13, 1, 7)")</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(13, 3, 3)")</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -693,10 +919,30 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (14,2,3,3)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (14, 2,3,3)");</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 1, 3)")</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 3, 3)")</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 4, 3)")</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 5, 5)")</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -720,10 +966,30 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (15,5,3,3)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (15, 5,3,3)");</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 1, 5)")</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 2, 3)")</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 3, 3)")</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 4, 3)")</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -744,10 +1010,30 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (16,1,3,4)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (16, 1,3,4)");</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 1, 3)")</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 2, 6)")</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 4, 3)")</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -768,10 +1054,30 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (17,2,3,4)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (17, 2,3,4)");</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 2, 3)")</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 4, 6)")</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -786,10 +1092,30 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (18,5,3,4)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (18, 5,3,4)");</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(18, 3, 7)")</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -807,10 +1133,30 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (19,5,3,5)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (19, 5,3,5)");</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(19, 3, 7)")</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(19, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -825,10 +1171,30 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (20,1,3,4)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (20, 1,3,4)");</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(20, 2, 7)")</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -849,10 +1215,30 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (21,4,3,4)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (21, 4,3,4)");</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 3, 3)")</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 4, 3)")</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 5, 6)")</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -870,10 +1256,30 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (22,2,3,5)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (22, 2,3,5)");</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(22, 2, 3)")</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(22, 4, 7)")</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -888,10 +1294,30 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (23,3,3,4)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (23, 3,3,4)");</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(23, 1, 7)")</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -915,10 +1341,30 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (24,1,3,3)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (24, 1,3,3)");</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 2, 3)")</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 3, 3)")</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 4, 5)")</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -942,10 +1388,30 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (25,4,3,3)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (25, 4,3,3)");</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 1, 3)")</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 2, 3)")</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 3, 5)")</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -960,10 +1426,30 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (26,2,3,4)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (26, 2,3,4)");</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(26, 4, 7)")</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -984,10 +1470,30 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (27,3,3,4)</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (27, 3,3,4)");</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 1, 6)")</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 2, 3)")</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 3, 3)")</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1002,10 +1508,30 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (28,4,3,4)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (28, 4,3,4)");</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(28, 5, 7)")</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1023,10 +1549,30 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (29,1,3,5)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (29, 1,3,5)");</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(29, 1, 3)")</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(29, 2, 7)")</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1047,10 +1593,30 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (30,5,3,4)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (30, 5,3,4)");</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 1, 3)")</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 3, 6)")</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1074,10 +1640,30 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (31,3,3,3)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (31, 3,3,3)");</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 1, 3)")</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 2, 5)")</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 4, 3)")</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1092,10 +1678,30 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (32,5,2,2)</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (32, 5,2,2)");</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(32, 1, 5)")</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1116,10 +1722,30 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (33,1,2,1)</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (33, 1,2,1)");</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 1, 2)")</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 3, 3)")</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 4, 3)")</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1140,10 +1766,30 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (34,5,2,1)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (34, 5,2,1)");</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 1, 2)")</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 2, 3)")</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 3, 2)")</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1164,10 +1810,30 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (35,5,2,2)</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (35, 5,2,2)");</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 1, 4)")</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 2, 1)")</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 3, 2)")</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1188,10 +1854,30 @@
       </c>
       <c r="I36" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (36,5,2,1)</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (36, 5,2,1)");</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 1, 3)")</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 4, 3)")</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1209,10 +1895,30 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (37,2,2,2)</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (37, 2,2,2)");</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(37, 2, 3)")</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(37, 4, 5)")</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1233,10 +1939,30 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (38,4,2,2)</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (38, 4,2,2)");</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 1, 1)")</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 3, 4)")</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1257,10 +1983,30 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (39,4,2,1)</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (39, 4,2,1)");</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 1, 3)")</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 2, 2)")</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 4, 2)")</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1281,10 +2027,30 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (40,2,2,2)</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (40, 2,2,2)");</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 3, 1)")</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 4, 2)")</v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 5, 4)")</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1299,10 +2065,30 @@
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (41,2,2,2)</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (41, 2,2,2)");</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(41, 2, 5)")</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1320,10 +2106,30 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (42,3,2,2)</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (42, 3,2,2)");</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(42, 1, 3)")</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(42, 2, 5)")</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1341,10 +2147,30 @@
       </c>
       <c r="I43" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (43,1,2,2)</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (43, 1,2,2)");</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(43, 3, 5)")</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(43, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1359,10 +2185,30 @@
       </c>
       <c r="I44" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (44,5,2,3)</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (44, 5,2,3)");</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(44, 5, 6)")</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1377,10 +2223,30 @@
       </c>
       <c r="I45" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (45,4,2,3)</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (45, 4,2,3)");</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(45, 4, 6)")</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1401,10 +2267,30 @@
       </c>
       <c r="I46" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (46,2,2,1)</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (46, 2,2,1)");</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 3, 2)")</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 4, 3)")</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1425,10 +2311,30 @@
       </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (47,3,2,1)</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (47, 3,2,1)");</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 2, 3)")</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 3, 2)")</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1443,10 +2349,30 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (48,1,2,3)</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (48, 1,2,3)");</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(48, 1, 6)")</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1467,10 +2393,30 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (49,4,2,1)</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (49, 4,2,1)");</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 2, 3)")</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 3, 3)")</v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 4, 2)")</v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1485,10 +2431,30 @@
       </c>
       <c r="I50" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (50,3,2,2)</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (50, 3,2,2)");</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(50, 5, 5)")</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1509,10 +2475,30 @@
       </c>
       <c r="I51" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (51,2,2,1)</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (51, 2,2,1)");</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 1, 3)")</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 2, 2)")</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -1527,10 +2513,30 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (52,4,2,2)</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (52, 4,2,2)");</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(52, 4, 5)")</v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -1551,10 +2557,30 @@
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (53,1,2,1)</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (53, 1,2,1)");</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 1, 2)")</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 3, 3)")</v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1569,10 +2595,30 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (54,1,2,2)</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (54, 1,2,2)");</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(54, 3, 5)")</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1593,10 +2639,30 @@
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (55,3,2,1)</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (55, 3,2,1)");</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 2, 2)")</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 4, 2)")</v>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1614,10 +2680,30 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (56,4,2,2)</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (56, 4,2,2)");</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(56, 4, 3)")</v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(56, 5, 5)")</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1638,10 +2724,30 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (57,3,2,2)</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (57, 3,2,2)");</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 1, 2)")</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 2, 4)")</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 4, 1)")</v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1662,10 +2768,30 @@
       </c>
       <c r="I58" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (58,1,2,2)</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (58, 1,2,2)");</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 2, 2)")</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 4, 4)")</v>
+      </c>
+      <c r="N58" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1683,10 +2809,30 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (59,5,2,2)</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (59, 5,2,2)");</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(59, 1, 5)")</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(59, 3, 3)")</v>
+      </c>
+      <c r="M59" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N59" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1701,10 +2847,30 @@
       </c>
       <c r="I60" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (60,2,2,3)</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (60, 2,2,3)");</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(60, 2, 6)")</v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1719,10 +2885,30 @@
       </c>
       <c r="I61" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (61,3,2,3)</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (61, 3,2,3)");</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(61, 3, 6)")</v>
+      </c>
+      <c r="M61" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -1742,11 +2928,31 @@
         <v>1</v>
       </c>
       <c r="I62" t="str">
-        <f>"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B62 &amp; "," &amp; A62 &amp; "," &amp; C62 &amp; ")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (62,3,1,0)</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (62, 3,1,0)");</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 1, 3)")</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 2, 1)")</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 3, 1)")</v>
+      </c>
+      <c r="M62" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1761,10 +2967,30 @@
       </c>
       <c r="I63" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (63,2,1,0)</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (63, 2,1,0)");</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(63, 1, 3)")</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M63" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -1785,10 +3011,30 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (64,1,1,0)</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (64, 1,1,0)");</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 1, 1)")</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 3, 3)")</v>
+      </c>
+      <c r="M64" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N64" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1</v>
       </c>
@@ -1809,10 +3055,30 @@
       </c>
       <c r="I65" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (65,5,1,0)</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (65, 5,1,0)");</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 3, 1)")</v>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 4, 1)")</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>
@@ -1836,10 +3102,30 @@
       </c>
       <c r="I66" t="str">
         <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (66,4,1,0)</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (66, 4,1,0)");</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="2"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 1, 2)")</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="3"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 2, 1)")</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 3, 1)")</v>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N66" t="str">
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1</v>
       </c>
@@ -1856,11 +3142,31 @@
         <v>1</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (67,5,1,0)</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I67:I101" si="7">"DoSqlRequest(""insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", "&amp;B67&amp;","&amp;A67&amp;","&amp;C67&amp;")"");"</f>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (67, 5,1,0)");</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J108" si="8">IF(ISBLANK(D67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D67),0,D67)&amp;")"")")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(67, 1, 2)")</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K108" si="9">IF(ISBLANK(E67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E67),0,E67)&amp;")"")")</f>
+        <v/>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" ref="L67:L108" si="10">IF(ISBLANK(F67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F67),0,F67)&amp;")"")")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(67, 3, 1)")</v>
+      </c>
+      <c r="M67" t="str">
+        <f t="shared" ref="M67:M108" si="11">IF(ISBLANK(G67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G67),0,G67)&amp;")"")")</f>
+        <v/>
+      </c>
+      <c r="N67" t="str">
+        <f t="shared" ref="N67:N108" si="12">IF(ISBLANK(H67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H67),0,H67)&amp;")"")")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1</v>
       </c>
@@ -1877,11 +3183,31 @@
         <v>2</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (68,5,1,0)</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (68, 5,1,0)");</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(68, 3, 2)")</v>
+      </c>
+      <c r="M68" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(68, 4, 2)")</v>
+      </c>
+      <c r="N68" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1</v>
       </c>
@@ -1895,11 +3221,31 @@
         <v>3</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (69,5,1,0)</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (69, 5,1,0)");</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M69" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(69, 4, 3)")</v>
+      </c>
+      <c r="N69" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1</v>
       </c>
@@ -1922,11 +3268,31 @@
         <v>1</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (70,5,1,0)</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (70, 5,1,0)");</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 1, 1)")</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 2, 2)")</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 3, 1)")</v>
+      </c>
+      <c r="M70" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 4, 1)")</v>
+      </c>
+      <c r="N70" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1</v>
       </c>
@@ -1946,11 +3312,31 @@
         <v>2</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (71,5,1,0)</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (71, 5,1,0)");</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 2, 2)")</v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 3, 1)")</v>
+      </c>
+      <c r="M71" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 4, 2)")</v>
+      </c>
+      <c r="N71" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -1973,11 +3359,31 @@
         <v>1</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (72,5,1,0)</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (72, 5,1,0)");</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 1, 1)")</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 2, 1)")</v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 3, 1)")</v>
+      </c>
+      <c r="M72" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 4, 1)")</v>
+      </c>
+      <c r="N72" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1</v>
       </c>
@@ -1991,11 +3397,31 @@
         <v>4</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (73,5,1,1)</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (73, 5,1,1)");</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(73, 2, 4)")</v>
+      </c>
+      <c r="L73" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M73" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N73" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -2018,11 +3444,31 @@
         <v>2</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (74,1,1,0)</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (74, 1,1,0)");</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 2, 1)")</v>
+      </c>
+      <c r="L74" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 3, 1)")</v>
+      </c>
+      <c r="M74" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 4, 1)")</v>
+      </c>
+      <c r="N74" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -2036,11 +3482,31 @@
         <v>3</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (75,1,1,0)</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (75, 1,1,0)");</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M75" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N75" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(75, 5, 3)")</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1</v>
       </c>
@@ -2057,11 +3523,31 @@
         <v>2</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (76,1,1,0)</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (76, 1,1,0)");</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(76, 1, 2)")</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L76" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M76" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N76" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(76, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -2078,11 +3564,31 @@
         <v>2</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" ref="I77:I101" si="2">"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B77 &amp; "," &amp; A77 &amp; "," &amp; C77 &amp; ")"</f>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (77,1,1,0)</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (77, 1,1,0)");</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(77, 2, 1)")</v>
+      </c>
+      <c r="L77" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M77" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(77, 4, 2)")</v>
+      </c>
+      <c r="N77" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -2102,11 +3608,31 @@
         <v>2</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (78,1,1,0)</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (78, 1,1,0)");</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 2, 1)")</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 3, 2)")</v>
+      </c>
+      <c r="M78" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N78" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1</v>
       </c>
@@ -2129,11 +3655,31 @@
         <v>1</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (79,1,1,0)</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (79, 1,1,0)");</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 2, 1)")</v>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 3, 1)")</v>
+      </c>
+      <c r="M79" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 4, 1)")</v>
+      </c>
+      <c r="N79" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -2147,11 +3693,31 @@
         <v>4</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (80,1,1,1)</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (80, 1,1,1)");</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L80" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M80" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N80" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(80, 5, 4)")</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
@@ -2171,11 +3737,31 @@
         <v>2</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (81,3,1,0)</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (81, 3,1,0)");</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 1, 1)")</v>
+      </c>
+      <c r="K81" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L81" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M81" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 4, 2)")</v>
+      </c>
+      <c r="N81" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -2192,11 +3778,31 @@
         <v>2</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (82,3,1,0)</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (82, 3,1,0)");</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(82, 2, 2)")</v>
+      </c>
+      <c r="L82" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M82" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N82" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(82, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1</v>
       </c>
@@ -2210,11 +3816,31 @@
         <v>3</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (83,3,1,0)</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (83, 3,1,0)");</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K83" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(83, 2, 3)")</v>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M83" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N83" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
@@ -2231,11 +3857,31 @@
         <v>2</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (84,3,1,0)</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (84, 3,1,0)");</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(84, 1, 1)")</v>
+      </c>
+      <c r="K84" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(84, 2, 2)")</v>
+      </c>
+      <c r="L84" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M84" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N84" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1</v>
       </c>
@@ -2258,11 +3904,31 @@
         <v>1</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (85,3,1,0)</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (85, 3,1,0)");</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 1, 1)")</v>
+      </c>
+      <c r="K85" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 2, 1)")</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M85" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 4, 1)")</v>
+      </c>
+      <c r="N85" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1</v>
       </c>
@@ -2285,11 +3951,31 @@
         <v>1</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (86,3,1,0)</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (86, 3,1,0)");</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 1, 1)")</v>
+      </c>
+      <c r="K86" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 2, 1)")</v>
+      </c>
+      <c r="L86" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M86" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 4, 2)")</v>
+      </c>
+      <c r="N86" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
@@ -2303,11 +3989,31 @@
         <v>4</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (87,3,1,1)</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (87, 3,1,1)");</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K87" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M87" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(87, 4, 4)")</v>
+      </c>
+      <c r="N87" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -2330,11 +4036,31 @@
         <v>1</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (88,4,1,0)</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (88, 4,1,0)");</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 1, 1)")</v>
+      </c>
+      <c r="K88" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 2, 1)")</v>
+      </c>
+      <c r="L88" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 3, 1)")</v>
+      </c>
+      <c r="M88" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N88" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
@@ -2351,11 +4077,31 @@
         <v>1</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (89,4,1,0)</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (89, 4,1,0)");</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K89" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L89" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(89, 3, 2)")</v>
+      </c>
+      <c r="M89" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N89" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(89, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -2369,11 +4115,31 @@
         <v>3</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (90,4,1,0)</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (90, 4,1,0)");</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K90" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L90" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(90, 3, 3)")</v>
+      </c>
+      <c r="M90" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N90" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1</v>
       </c>
@@ -2393,11 +4159,31 @@
         <v>1</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (91,4,1,0)</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (91, 4,1,0)");</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 1, 2)")</v>
+      </c>
+      <c r="K91" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 2, 2)")</v>
+      </c>
+      <c r="L91" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M91" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N91" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -2414,11 +4200,31 @@
         <v>2</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (92,4,1,0)</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (92, 4,1,0)");</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K92" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(92, 2, 2)")</v>
+      </c>
+      <c r="L92" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(92, 3, 2)")</v>
+      </c>
+      <c r="M92" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N92" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -2438,11 +4244,31 @@
         <v>1</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (93,4,1,0)</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (93, 4,1,0)");</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 1, 1)")</v>
+      </c>
+      <c r="K93" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 2, 3)")</v>
+      </c>
+      <c r="L93" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M93" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 4, 1)")</v>
+      </c>
+      <c r="N93" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -2456,11 +4282,31 @@
         <v>4</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (94,4,1,1)</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (94, 4,1,1)");</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(94, 1, 4)")</v>
+      </c>
+      <c r="K94" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L94" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M94" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N94" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>
@@ -2480,11 +4326,31 @@
         <v>1</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (95,2,1,0)</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (95, 2,1,0)");</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K95" t="str">
+        <f t="shared" si="9"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 2, 1)")</v>
+      </c>
+      <c r="L95" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M95" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 4, 3)")</v>
+      </c>
+      <c r="N95" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2504,11 +4370,31 @@
         <v>1</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (96,2,1,0)</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (96, 2,1,0)");</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 1, 2)")</v>
+      </c>
+      <c r="K96" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L96" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 3, 2)")</v>
+      </c>
+      <c r="M96" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 4, 1)")</v>
+      </c>
+      <c r="N96" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
@@ -2531,11 +4417,31 @@
         <v>1</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (97,2,1,0)</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (97, 2,1,0)");</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 1, 1)")</v>
+      </c>
+      <c r="K97" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L97" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 3, 1)")</v>
+      </c>
+      <c r="M97" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 4, 1)")</v>
+      </c>
+      <c r="N97" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1</v>
       </c>
@@ -2552,11 +4458,31 @@
         <v>2</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (98,2,1,0)</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (98, 2,1,0)");</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(98, 1, 2)")</v>
+      </c>
+      <c r="K98" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L98" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M98" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(98, 4, 2)")</v>
+      </c>
+      <c r="N98" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1</v>
       </c>
@@ -2573,11 +4499,31 @@
         <v>2</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (99,2,1,0)</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (99, 2,1,0)");</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K99" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L99" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M99" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(99, 4, 1)")</v>
+      </c>
+      <c r="N99" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(99, 5, 2)")</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1</v>
       </c>
@@ -2600,11 +4546,31 @@
         <v>1</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (100,2,1,0)</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (100, 2,1,0)");</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="8"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 1, 1)")</v>
+      </c>
+      <c r="K100" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L100" t="str">
+        <f t="shared" si="10"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 3, 2)")</v>
+      </c>
+      <c r="M100" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 4, 1)")</v>
+      </c>
+      <c r="N100" t="str">
+        <f t="shared" si="12"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 5, 1)")</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1</v>
       </c>
@@ -2618,8 +4584,182 @@
         <v>4</v>
       </c>
       <c r="I101" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (101,2,1,1)</v>
+        <f t="shared" si="7"/>
+        <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (101, 2,1,1)");</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K101" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L101" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M101" t="str">
+        <f t="shared" si="11"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(101, 4, 4)")</v>
+      </c>
+      <c r="N101" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J102" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K102" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L102" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M102" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N102" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J103" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K103" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L103" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M103" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N103" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J104" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K104" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L104" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M104" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N104" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J105" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K105" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L105" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M105" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N105" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J106" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K106" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L106" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M106" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N106" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J107" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K107" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L107" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M107" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N107" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J108" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K108" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L108" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M108" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N108" t="str">
+        <f t="shared" si="12"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changement mineurs sur la sélection de données
</commit_message>
<xml_diff>
--- a/MLD & cartes/Splendor_Cartes - sans requetes.xlsx
+++ b/MLD & cartes/Splendor_Cartes - sans requetes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,9 +368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J100" sqref="J100"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -436,20 +436,20 @@
         <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (2, ,4,3)");</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(ISBLANK(D2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D2),0,D2)&amp;")"")")</f>
+        <f>IF(ISBLANK(D2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D2),0,D2)&amp;")"");")</f>
         <v/>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:N2" si="0">IF(ISBLANK(E2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E2),0,E2)&amp;")"")")</f>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(2, 2, 4)")</v>
+        <f>IF(ISBLANK(E2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E2),0,E2)&amp;")"");")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(2, 2, 4)");</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L2:N17" si="0">IF(ISBLANK(F2),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F2),0,F2)&amp;")"");")</f>
         <v/>
       </c>
       <c r="M2" t="str">
         <f t="shared" si="0"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(2, 4, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(2, 4, 4)");</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" si="0"/>
@@ -474,23 +474,23 @@
         <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (3, ,4,3)");</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J66" si="2">IF(ISBLANK(D3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D3),0,D3)&amp;")"")")</f>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(3, 1, 4)")</v>
+        <f t="shared" ref="J3:J66" si="2">IF(ISBLANK(D3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D3),0,D3)&amp;")"");")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(3, 1, 4)");</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K66" si="3">IF(ISBLANK(E3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E3),0,E3)&amp;")"")")</f>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(3, 2, 4)")</v>
+        <f t="shared" ref="K3:K66" si="3">IF(ISBLANK(E3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E3),0,E3)&amp;")"");")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(3, 2, 4)");</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L66" si="4">IF(ISBLANK(F3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F3),0,F3)&amp;")"")")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M66" si="5">IF(ISBLANK(G3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G3),0,G3)&amp;")"")")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N66" si="6">IF(ISBLANK(H3),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H3),0,H3)&amp;")"")")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -523,16 +523,16 @@
         <v/>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 3, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 3, 3)");</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 4, 3)");</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 5, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(4, 5, 3)");</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -561,16 +561,16 @@
         <v/>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(5, 3, 4)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(5, 3, 4)");</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(5, 5, 4)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(5, 5, 4)");</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -592,22 +592,22 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(6, 1, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(6, 1, 4)");</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(6, 3, 4)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(6, 3, 4)");</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -633,23 +633,23 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 1, 3)");</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 3, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 3, 3)");</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 5, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(7, 5, 3)");</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -678,19 +678,19 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 2, 3)");</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 4, 3)");</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 5, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(8, 5, 3)");</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -715,22 +715,22 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 1, 3)");</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 2, 3)");</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(9, 4, 3)");</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -760,16 +760,16 @@
         <v/>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(10, 4, 4)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(10, 4, 4)");</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(10, 5, 4)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(10, 5, 4)");</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -794,22 +794,22 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 1, 3)");</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 2, 3)");</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 3, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(11, 3, 3)");</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -842,16 +842,16 @@
         <v/>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(12, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(12, 4, 3)");</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(12, 5, 7)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(12, 5, 7)");</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -876,22 +876,22 @@
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(13, 1, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(13, 1, 7)");</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(13, 3, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(13, 3, 3)");</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -923,23 +923,23 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 1, 3)");</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 3, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 3, 3)");</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 4, 3)");</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 5, 5)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(14, 5, 5)");</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -970,22 +970,22 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 1, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 1, 5)");</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 2, 3)");</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 3, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 3, 3)");</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(15, 4, 3)");</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1014,22 +1014,22 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 1, 3)");</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 2, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 2, 6)");</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 4, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(16, 4, 3)");</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1062,19 +1062,19 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 2, 3)");</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 4, 6)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 4, 6)");</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 5, 3)")</v>
+        <f t="shared" si="0"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(17, 5, 3)");</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1103,15 +1103,15 @@
         <v/>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(18, 3, 7)")</v>
+        <f t="shared" ref="L18:L81" si="4">IF(ISBLANK(F18),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F18),0,F18)&amp;")"");")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(18, 3, 7)");</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M18:M81" si="5">IF(ISBLANK(G18),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G18),0,G18)&amp;")"");")</f>
         <v/>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="N18:N81" si="6">IF(ISBLANK(H18),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H18),0,H18)&amp;")"");")</f>
         <v/>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(19, 3, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(19, 3, 7)");</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="5"/>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="N19" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(19, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(19, 5, 3)");</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(20, 2, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(20, 2, 7)");</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="4"/>
@@ -1227,15 +1227,15 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 3, 3)");</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 4, 3)");</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 5, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(21, 5, 6)");</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(22, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(22, 2, 3)");</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="4"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(22, 4, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(22, 4, 7)");</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="6"/>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(23, 1, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(23, 1, 7)");</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="3"/>
@@ -1349,19 +1349,19 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 2, 3)");</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 3, 3)");</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 4, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 4, 5)");</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(24, 5, 3)");</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1392,15 +1392,15 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 1, 3)");</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 2, 3)");</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 3, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 3, 5)");</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="5"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="N25" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(25, 5, 3)");</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(26, 4, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(26, 4, 7)");</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="6"/>
@@ -1474,15 +1474,15 @@
       </c>
       <c r="J27" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 1, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 1, 6)");</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 2, 3)");</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(27, 3, 3)");</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="5"/>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="N28" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(28, 5, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(28, 5, 7)");</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1553,11 +1553,11 @@
       </c>
       <c r="J29" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(29, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(29, 1, 3)");</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(29, 2, 7)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(29, 2, 7)");</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="4"/>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 1, 3)");</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="3"/>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="L30" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 3, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 3, 6)");</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="5"/>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(30, 5, 3)");</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -1644,11 +1644,11 @@
       </c>
       <c r="J31" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 1, 3)");</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 2, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 2, 5)");</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="4"/>
@@ -1656,11 +1656,11 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 4, 3)");</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(31, 5, 3)");</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="J32" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(32, 1, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(32, 1, 5)");</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="3"/>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="J33" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 1, 2)");</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="3"/>
@@ -1734,11 +1734,11 @@
       </c>
       <c r="L33" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 3, 3)");</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(33, 4, 3)");</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="6"/>
@@ -1770,15 +1770,15 @@
       </c>
       <c r="J34" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 1, 2)");</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 2, 3)");</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(34, 3, 2)");</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="5"/>
@@ -1814,15 +1814,15 @@
       </c>
       <c r="J35" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 1, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 1, 4)");</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 2, 1)");</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(35, 3, 2)");</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="5"/>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="J36" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 1, 3)");</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="3"/>
@@ -1870,11 +1870,11 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 4, 3)");</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 5, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(36, 5, 2)");</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="K37" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(37, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(37, 2, 3)");</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="4"/>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(37, 4, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(37, 4, 5)");</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="6"/>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 1, 1)");</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="3"/>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="L38" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 3, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 3, 4)");</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="N38" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 5, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(38, 5, 2)");</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -1987,11 +1987,11 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 1, 3)");</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 2, 2)");</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="4"/>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 4, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(39, 4, 2)");</v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="6"/>
@@ -2039,15 +2039,15 @@
       </c>
       <c r="L40" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 3, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 3, 1)");</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 4, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 4, 2)");</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 5, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(40, 5, 4)");</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="K41" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(41, 2, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(41, 2, 5)");</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="4"/>
@@ -2110,11 +2110,11 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(42, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(42, 1, 3)");</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(42, 2, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(42, 2, 5)");</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="4"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="L43" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(43, 3, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(43, 3, 5)");</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="N43" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(43, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(43, 5, 3)");</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="N44" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(44, 5, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(44, 5, 6)");</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="M45" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(45, 4, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(45, 4, 6)");</v>
       </c>
       <c r="N45" t="str">
         <f t="shared" si="6"/>
@@ -2279,15 +2279,15 @@
       </c>
       <c r="L46" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 3, 2)");</v>
       </c>
       <c r="M46" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 4, 3)");</v>
       </c>
       <c r="N46" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 5, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(46, 5, 2)");</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -2319,11 +2319,11 @@
       </c>
       <c r="K47" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 2, 3)");</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 3, 2)");</v>
       </c>
       <c r="M47" t="str">
         <f t="shared" si="5"/>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="N47" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(47, 5, 3)");</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="J48" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(48, 1, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(48, 1, 6)");</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="3"/>
@@ -2401,15 +2401,15 @@
       </c>
       <c r="K49" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 2, 3)");</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 3, 3)");</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 4, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(49, 4, 2)");</v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="6"/>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="N50" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(50, 5, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(50, 5, 5)");</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="J51" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 1, 3)");</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 2, 2)");</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="4"/>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="N51" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(51, 5, 3)");</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="M52" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(52, 4, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(52, 4, 5)");</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="6"/>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="J53" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 1, 2)");</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="3"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="L53" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 3, 3)");</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="5"/>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="N53" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 5, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(53, 5, 2)");</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="L54" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(54, 3, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(54, 3, 5)");</v>
       </c>
       <c r="M54" t="str">
         <f t="shared" si="5"/>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="K55" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 2, 2)");</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="4"/>
@@ -2655,11 +2655,11 @@
       </c>
       <c r="M55" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 4, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 4, 2)");</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(55, 5, 3)");</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -2696,11 +2696,11 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(56, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(56, 4, 3)");</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(56, 5, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(56, 5, 5)");</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -2728,11 +2728,11 @@
       </c>
       <c r="J57" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 1, 2)");</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 2, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 2, 4)");</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="4"/>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(57, 4, 1)");</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="6"/>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="K58" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 2, 2)");</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="4"/>
@@ -2784,11 +2784,11 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 4, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 4, 4)");</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(58, 5, 1)");</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="J59" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(59, 1, 5)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(59, 1, 5)");</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="3"/>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="L59" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(59, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(59, 3, 3)");</v>
       </c>
       <c r="M59" t="str">
         <f t="shared" si="5"/>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="K60" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(60, 2, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(60, 2, 6)");</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" si="4"/>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="L61" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(61, 3, 6)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(61, 3, 6)");</v>
       </c>
       <c r="M61" t="str">
         <f t="shared" si="5"/>
@@ -2933,15 +2933,15 @@
       </c>
       <c r="J62" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 1, 3)");</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 2, 1)");</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 3, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(62, 3, 1)");</v>
       </c>
       <c r="M62" t="str">
         <f t="shared" si="5"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="J63" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(63, 1, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(63, 1, 3)");</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="3"/>
@@ -3015,7 +3015,7 @@
       </c>
       <c r="J64" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 1, 1)");</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="3"/>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="L64" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 3, 3)");</v>
       </c>
       <c r="M64" t="str">
         <f t="shared" si="5"/>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="N64" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(64, 5, 1)");</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -3067,15 +3067,15 @@
       </c>
       <c r="L65" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 3, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 3, 1)");</v>
       </c>
       <c r="M65" t="str">
         <f t="shared" si="5"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 4, 1)");</v>
       </c>
       <c r="N65" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 5, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(65, 5, 3)");</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -3106,15 +3106,15 @@
       </c>
       <c r="J66" t="str">
         <f t="shared" si="2"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 1, 2)");</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="3"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 2, 1)");</v>
       </c>
       <c r="L66" t="str">
         <f t="shared" si="4"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 3, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 3, 1)");</v>
       </c>
       <c r="M66" t="str">
         <f t="shared" si="5"/>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="N66" t="str">
         <f t="shared" si="6"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(66, 5, 1)");</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -3146,23 +3146,23 @@
         <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (67, 5,1,0)");</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J108" si="8">IF(ISBLANK(D67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D67),0,D67)&amp;")"")")</f>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(67, 1, 2)")</v>
+        <f t="shared" ref="J67:J100" si="8">IF(ISBLANK(D67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D67),0,D67)&amp;")"");")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(67, 1, 2)");</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K108" si="9">IF(ISBLANK(E67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E67),0,E67)&amp;")"")")</f>
+        <f t="shared" ref="K67:K100" si="9">IF(ISBLANK(E67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E67),0,E67)&amp;")"");")</f>
         <v/>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L108" si="10">IF(ISBLANK(F67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F67),0,F67)&amp;")"")")</f>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(67, 3, 1)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(67, 3, 1)");</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" ref="M67:M108" si="11">IF(ISBLANK(G67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G67),0,G67)&amp;")"")")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N67" t="str">
-        <f t="shared" ref="N67:N108" si="12">IF(ISBLANK(H67),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H67),0,H67)&amp;")"")")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3195,15 +3195,15 @@
         <v/>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(68, 3, 2)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(68, 3, 2)");</v>
       </c>
       <c r="M68" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(68, 4, 2)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(68, 4, 2)");</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3233,15 +3233,15 @@
         <v/>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M69" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(69, 4, 3)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(69, 4, 3)");</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3273,22 +3273,22 @@
       </c>
       <c r="J70" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 1, 1)");</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 2, 2)");</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 3, 1)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 3, 1)");</v>
       </c>
       <c r="M70" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 4, 1)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(70, 4, 1)");</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3321,18 +3321,18 @@
       </c>
       <c r="K71" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 2, 2)");</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 3, 1)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 3, 1)");</v>
       </c>
       <c r="M71" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 4, 2)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(71, 4, 2)");</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3364,22 +3364,22 @@
       </c>
       <c r="J72" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 1, 1)");</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 2, 1)");</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 3, 1)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 3, 1)");</v>
       </c>
       <c r="M72" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 4, 1)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(72, 4, 1)");</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3406,18 +3406,18 @@
       </c>
       <c r="K73" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(73, 2, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(73, 2, 4)");</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M73" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3453,19 +3453,19 @@
       </c>
       <c r="K74" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 2, 1)");</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 3, 1)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 3, 1)");</v>
       </c>
       <c r="M74" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 4, 1)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 4, 1)");</v>
       </c>
       <c r="N74" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 5, 2)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(74, 5, 2)");</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -3494,16 +3494,16 @@
         <v/>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(75, 5, 3)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(75, 5, 3)");</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -3528,23 +3528,23 @@
       </c>
       <c r="J76" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(76, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(76, 1, 2)");</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="L76" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N76" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(76, 5, 2)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(76, 5, 2)");</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -3573,18 +3573,18 @@
       </c>
       <c r="K77" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(77, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(77, 2, 1)");</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M77" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(77, 4, 2)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(77, 4, 2)");</v>
       </c>
       <c r="N77" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3617,19 +3617,19 @@
       </c>
       <c r="K78" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 2, 1)");</v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 3, 2)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 3, 2)");</v>
       </c>
       <c r="M78" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N78" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 5, 2)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(78, 5, 2)");</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -3664,19 +3664,19 @@
       </c>
       <c r="K79" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 2, 1)");</v>
       </c>
       <c r="L79" t="str">
-        <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 3, 1)")</v>
+        <f t="shared" si="4"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 3, 1)");</v>
       </c>
       <c r="M79" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 4, 1)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 4, 1)");</v>
       </c>
       <c r="N79" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 5, 1)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(79, 5, 1)");</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -3705,16 +3705,16 @@
         <v/>
       </c>
       <c r="L80" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N80" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(80, 5, 4)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(80, 5, 4)");</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -3742,23 +3742,23 @@
       </c>
       <c r="J81" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 1, 1)");</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M81" t="str">
-        <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 4, 2)")</v>
+        <f t="shared" si="5"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 4, 2)");</v>
       </c>
       <c r="N81" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 5, 2)")</v>
+        <f t="shared" si="6"/>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(81, 5, 2)");</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -3787,19 +3787,19 @@
       </c>
       <c r="K82" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(82, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(82, 2, 2)");</v>
       </c>
       <c r="L82" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="L82:L100" si="10">IF(ISBLANK(F82),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F82),0,F82)&amp;")"");")</f>
         <v/>
       </c>
       <c r="M82" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M82:M100" si="11">IF(ISBLANK(G82),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G82),0,G82)&amp;")"");")</f>
         <v/>
       </c>
       <c r="N82" t="str">
-        <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(82, 5, 2)")</v>
+        <f t="shared" ref="N82:N100" si="12">IF(ISBLANK(H82),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H82),0,H82)&amp;")"");")</f>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(82, 5, 2)");</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="K83" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(83, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(83, 2, 3)");</v>
       </c>
       <c r="L83" t="str">
         <f t="shared" si="10"/>
@@ -3862,11 +3862,11 @@
       </c>
       <c r="J84" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(84, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(84, 1, 1)");</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(84, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(84, 2, 2)");</v>
       </c>
       <c r="L84" t="str">
         <f t="shared" si="10"/>
@@ -3909,11 +3909,11 @@
       </c>
       <c r="J85" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 1, 1)");</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 2, 1)");</v>
       </c>
       <c r="L85" t="str">
         <f t="shared" si="10"/>
@@ -3921,11 +3921,11 @@
       </c>
       <c r="M85" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 4, 1)");</v>
       </c>
       <c r="N85" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(85, 5, 1)");</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -3956,11 +3956,11 @@
       </c>
       <c r="J86" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 1, 1)");</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 2, 1)");</v>
       </c>
       <c r="L86" t="str">
         <f t="shared" si="10"/>
@@ -3968,11 +3968,11 @@
       </c>
       <c r="M86" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 4, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 4, 2)");</v>
       </c>
       <c r="N86" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(86, 5, 1)");</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="M87" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(87, 4, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(87, 4, 4)");</v>
       </c>
       <c r="N87" t="str">
         <f t="shared" si="12"/>
@@ -4041,15 +4041,15 @@
       </c>
       <c r="J88" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 1, 1)");</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 2, 1)");</v>
       </c>
       <c r="L88" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 3, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 3, 1)");</v>
       </c>
       <c r="M88" t="str">
         <f t="shared" si="11"/>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="N88" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(88, 5, 1)");</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="L89" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(89, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(89, 3, 2)");</v>
       </c>
       <c r="M89" t="str">
         <f t="shared" si="11"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="N89" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(89, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(89, 5, 1)");</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -4128,7 +4128,7 @@
       </c>
       <c r="L90" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(90, 3, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(90, 3, 3)");</v>
       </c>
       <c r="M90" t="str">
         <f t="shared" si="11"/>
@@ -4164,11 +4164,11 @@
       </c>
       <c r="J91" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 1, 2)");</v>
       </c>
       <c r="K91" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 2, 2)");</v>
       </c>
       <c r="L91" t="str">
         <f t="shared" si="10"/>
@@ -4180,7 +4180,7 @@
       </c>
       <c r="N91" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(91, 5, 1)");</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -4209,11 +4209,11 @@
       </c>
       <c r="K92" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(92, 2, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(92, 2, 2)");</v>
       </c>
       <c r="L92" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(92, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(92, 3, 2)");</v>
       </c>
       <c r="M92" t="str">
         <f t="shared" si="11"/>
@@ -4249,11 +4249,11 @@
       </c>
       <c r="J93" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 1, 1)");</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 2, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 2, 3)");</v>
       </c>
       <c r="L93" t="str">
         <f t="shared" si="10"/>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="M93" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(93, 4, 1)");</v>
       </c>
       <c r="N93" t="str">
         <f t="shared" si="12"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="J94" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(94, 1, 4)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(94, 1, 4)");</v>
       </c>
       <c r="K94" t="str">
         <f t="shared" si="9"/>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="K95" t="str">
         <f t="shared" si="9"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 2, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 2, 1)");</v>
       </c>
       <c r="L95" t="str">
         <f t="shared" si="10"/>
@@ -4343,11 +4343,11 @@
       </c>
       <c r="M95" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 4, 3)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 4, 3)");</v>
       </c>
       <c r="N95" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(95, 5, 1)");</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -4375,7 +4375,7 @@
       </c>
       <c r="J96" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 1, 2)");</v>
       </c>
       <c r="K96" t="str">
         <f t="shared" si="9"/>
@@ -4383,11 +4383,11 @@
       </c>
       <c r="L96" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 3, 2)");</v>
       </c>
       <c r="M96" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(96, 4, 1)");</v>
       </c>
       <c r="N96" t="str">
         <f t="shared" si="12"/>
@@ -4422,7 +4422,7 @@
       </c>
       <c r="J97" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 1, 1)");</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="9"/>
@@ -4430,15 +4430,15 @@
       </c>
       <c r="L97" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 3, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 3, 1)");</v>
       </c>
       <c r="M97" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 4, 1)");</v>
       </c>
       <c r="N97" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(97, 5, 1)");</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="J98" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(98, 1, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(98, 1, 2)");</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="9"/>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="M98" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(98, 4, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(98, 4, 2)");</v>
       </c>
       <c r="N98" t="str">
         <f t="shared" si="12"/>
@@ -4516,11 +4516,11 @@
       </c>
       <c r="M99" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(99, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(99, 4, 1)");</v>
       </c>
       <c r="N99" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(99, 5, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(99, 5, 2)");</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="J100" t="str">
         <f t="shared" si="8"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 1, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 1, 1)");</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="9"/>
@@ -4559,15 +4559,15 @@
       </c>
       <c r="L100" t="str">
         <f t="shared" si="10"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 3, 2)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 3, 2)");</v>
       </c>
       <c r="M100" t="str">
         <f t="shared" si="11"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 4, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 4, 1)");</v>
       </c>
       <c r="N100" t="str">
         <f t="shared" si="12"/>
-        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 5, 1)")</v>
+        <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(100, 5, 1)");</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -4588,177 +4588,177 @@
         <v>DoSqlRequest("insert into card(idcard, fkRessource, level, nbPtPrestige) values (101, 2,1,1)");</v>
       </c>
       <c r="J101" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="J67:J108" si="13">IF(ISBLANK(D101),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;D$1&amp;", "&amp;IF(ISBLANK(D101),0,D101)&amp;")"")")</f>
         <v/>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="K67:K108" si="14">IF(ISBLANK(E101),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;E$1&amp;", "&amp;IF(ISBLANK(E101),0,E101)&amp;")"")")</f>
         <v/>
       </c>
       <c r="L101" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="L67:L108" si="15">IF(ISBLANK(F101),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;F$1&amp;", "&amp;IF(ISBLANK(F101),0,F101)&amp;")"")")</f>
         <v/>
       </c>
       <c r="M101" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M67:M108" si="16">IF(ISBLANK(G101),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;G$1&amp;", "&amp;IF(ISBLANK(G101),0,G101)&amp;")"")")</f>
         <v>DoSqlRequest("Insert into Cost(fkCard, fkRessource, nbRessource) values(101, 4, 4)")</v>
       </c>
       <c r="N101" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="N67:N108" si="17">IF(ISBLANK(H101),"","DoSqlRequest(""Insert into Cost(fkCard, fkRessource, nbRessource) values("&amp;ROW()&amp;", "&amp;H$1&amp;", "&amp;IF(ISBLANK(H101),0,H101)&amp;")"")")</f>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J102" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L102" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M102" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N102" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J103" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L103" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M103" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N103" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J104" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L104" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M104" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N104" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J105" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L105" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M105" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N105" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J106" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L106" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M106" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N106" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J107" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L107" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M107" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N107" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J108" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M108" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N108" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>

</xml_diff>